<commit_message>
Sprint 8 - Quase pronta
</commit_message>
<xml_diff>
--- a/Sprint 8/Product Backlog-Burndown.xlsx
+++ b/Sprint 8/Product Backlog-Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI\4-Periodo\PDS\SistemaC\SistemaC\Sprint 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="192">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -358,15 +358,6 @@
     <t>Inserção de JComboBox com dados de cidades e estados nas telas de cadastro</t>
   </si>
   <si>
-    <t>inserção de metodos de agendamento no bando de dados</t>
-  </si>
-  <si>
-    <t>inserção de metodos de busca de agedamentos no banco de dados</t>
-  </si>
-  <si>
-    <t>inserção de metodos de controle de horários no banco de dados</t>
-  </si>
-  <si>
     <t>Atualização MVC</t>
   </si>
   <si>
@@ -470,6 +461,147 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>Melhoramento do Módulo Prontuário</t>
+  </si>
+  <si>
+    <t>Tela de Informações do paciente</t>
+  </si>
+  <si>
+    <t>Análise do projeto</t>
+  </si>
+  <si>
+    <t>Remoção de classes desnecessárias</t>
+  </si>
+  <si>
+    <t>Inserção de métodos e atributos</t>
+  </si>
+  <si>
+    <t>Melhoramento na codificação de busca de prontuário</t>
+  </si>
+  <si>
+    <t>Melhoramento codificação de alteração de prontuário</t>
+  </si>
+  <si>
+    <t>Inserção de atributos na classe protuário</t>
+  </si>
+  <si>
+    <t>Mudança nos métodos de acesso ao prontuário</t>
+  </si>
+  <si>
+    <t>Melhoramento na integração com agendamento</t>
+  </si>
+  <si>
+    <t>Analise do banco de dados</t>
+  </si>
+  <si>
+    <t>Recriação do banco de dados</t>
+  </si>
+  <si>
+    <t>Criação de diagramas do banco de dados</t>
+  </si>
+  <si>
+    <t>Criação de script para esquema do banco de dados</t>
+  </si>
+  <si>
+    <t>Criação de método cadastro de paciente</t>
+  </si>
+  <si>
+    <t>Criação de método consulta de paciente</t>
+  </si>
+  <si>
+    <t>Criação de método alteração de paciente</t>
+  </si>
+  <si>
+    <t>Teste de inserção e consulta de paciente</t>
+  </si>
+  <si>
+    <t>Criação de método cadastro de funcionário</t>
+  </si>
+  <si>
+    <t>Criação de método consulta de funcionario</t>
+  </si>
+  <si>
+    <t>Criação de método alteração de funcionário</t>
+  </si>
+  <si>
+    <t>Teste de inserção e consulta de funcionario</t>
+  </si>
+  <si>
+    <t>Criação de método cadastro de agenda</t>
+  </si>
+  <si>
+    <t>Criação de método consulta de agenda</t>
+  </si>
+  <si>
+    <t>Criação de método alteração de agenda</t>
+  </si>
+  <si>
+    <t>Teste de inserção e consulta de agenda</t>
+  </si>
+  <si>
+    <t>Criação de método para criação de prontuário de atendimento</t>
+  </si>
+  <si>
+    <t>Criação de método para consulta de prontuário de atendimento</t>
+  </si>
+  <si>
+    <t>Criação de método para alteração de prontuário de atendimento</t>
+  </si>
+  <si>
+    <t>Teste de inserção de consulta de prontuário</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de cadastro de paciente</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de cadastro de funcionário</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de busca de paciente</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de busca de funcionário</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de alteração de paciente</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de alteração de funcionário</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de remoção de paciente</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de remoção de funcionário</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de agendamento de consulta</t>
+  </si>
+  <si>
+    <t>Integração com a funcionalidade de busca de agendamentos</t>
+  </si>
+  <si>
+    <t>Implementação de métodos e atributos</t>
+  </si>
+  <si>
+    <t>Integração com o sistema</t>
+  </si>
+  <si>
+    <t>Atualizar diagrama de entidade relacionamento</t>
+  </si>
+  <si>
+    <t>Melhoramento de funcionalidades</t>
+  </si>
+  <si>
+    <t>Alterações de métodos</t>
+  </si>
+  <si>
+    <t>Testes e implementações</t>
+  </si>
+  <si>
+    <t>Codificação de métodos e parte gráfica</t>
   </si>
 </sst>
 </file>
@@ -784,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -909,20 +1041,62 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -932,56 +1106,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,9 +1128,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1246,7 +1372,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1370,13 +1496,13 @@
                   <c:v>271.27</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>271.27</c:v>
+                  <c:v>226.51999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>271.27</c:v>
+                  <c:v>226.51999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>271.27</c:v>
+                  <c:v>226.51999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1390,7 +1516,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1456,11 +1582,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145765296"/>
-        <c:axId val="145764904"/>
+        <c:axId val="245197920"/>
+        <c:axId val="245198312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145765296"/>
+        <c:axId val="245197920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1621,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145764904"/>
+        <c:crossAx val="245198312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1503,7 +1629,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145764904"/>
+        <c:axId val="245198312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1549,7 +1675,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145765296"/>
+        <c:crossAx val="245197920"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1930,10 +2056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S99"/>
+  <dimension ref="A1:S137"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1948,14 +2074,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2159,10 +2285,10 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="58" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -2192,8 +2318,8 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="68"/>
-      <c r="B9" s="70"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="23" t="s">
         <v>43</v>
       </c>
@@ -2221,8 +2347,8 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68"/>
-      <c r="B10" s="70"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="23" t="s">
         <v>44</v>
       </c>
@@ -2250,8 +2376,8 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="68"/>
-      <c r="B11" s="70"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="23" t="s">
         <v>45</v>
       </c>
@@ -2279,8 +2405,8 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="68"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="23" t="s">
         <v>46</v>
       </c>
@@ -2308,8 +2434,8 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="68"/>
-      <c r="B13" s="70"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="23" t="s">
         <v>47</v>
       </c>
@@ -2337,8 +2463,8 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="68"/>
-      <c r="B14" s="71"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="23" t="s">
         <v>48</v>
       </c>
@@ -2366,10 +2492,10 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="23" t="s">
@@ -2399,8 +2525,8 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="66"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="24" t="s">
         <v>52</v>
       </c>
@@ -2428,8 +2554,8 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="66"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="24" t="s">
         <v>54</v>
       </c>
@@ -2457,8 +2583,8 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="65"/>
-      <c r="B18" s="60"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="25" t="s">
         <v>53</v>
       </c>
@@ -2486,10 +2612,10 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="50" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="22" t="s">
@@ -2519,8 +2645,8 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="65"/>
-      <c r="B20" s="60"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="23" t="s">
         <v>73</v>
       </c>
@@ -2548,10 +2674,10 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="50" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="22" t="s">
@@ -2581,8 +2707,8 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="65"/>
-      <c r="B22" s="60"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="23" t="s">
         <v>73</v>
       </c>
@@ -2610,10 +2736,10 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="50" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="22" t="s">
@@ -2643,8 +2769,8 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="65"/>
-      <c r="B24" s="60"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="23" t="s">
         <v>73</v>
       </c>
@@ -2672,10 +2798,10 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="50" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="22" t="s">
@@ -2705,8 +2831,8 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="65"/>
-      <c r="B26" s="60"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="23" t="s">
         <v>73</v>
       </c>
@@ -2734,10 +2860,10 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="61" t="s">
         <v>77</v>
       </c>
       <c r="C27" s="22" t="s">
@@ -2767,8 +2893,8 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="65"/>
-      <c r="B28" s="57"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="62"/>
       <c r="C28" s="22" t="s">
         <v>75</v>
       </c>
@@ -2796,10 +2922,10 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="58" t="s">
+      <c r="A29" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="50" t="s">
         <v>89</v>
       </c>
       <c r="C29" s="33" t="s">
@@ -2829,8 +2955,8 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
+      <c r="A30" s="51"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="38" t="s">
         <v>81</v>
       </c>
@@ -2858,10 +2984,10 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="50" t="s">
         <v>90</v>
       </c>
       <c r="C31" s="39" t="s">
@@ -2891,8 +3017,8 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="40" t="s">
         <v>83</v>
       </c>
@@ -2920,8 +3046,8 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="41" t="s">
         <v>84</v>
       </c>
@@ -2949,8 +3075,8 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="42" t="s">
         <v>85</v>
       </c>
@@ -2978,8 +3104,8 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="60"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="42" t="s">
         <v>86</v>
       </c>
@@ -3007,10 +3133,10 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="50" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="39" t="s">
@@ -3040,8 +3166,8 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="60"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="39" t="s">
         <v>88</v>
       </c>
@@ -3069,10 +3195,10 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="61" t="s">
+      <c r="A38" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="58"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="33" t="s">
         <v>96</v>
       </c>
@@ -3100,8 +3226,8 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="62"/>
-      <c r="B39" s="59"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="38" t="s">
         <v>97</v>
       </c>
@@ -3129,8 +3255,8 @@
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="63"/>
-      <c r="B40" s="60"/>
+      <c r="A40" s="65"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="39" t="s">
         <v>98</v>
       </c>
@@ -3158,10 +3284,10 @@
       <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="50" t="s">
         <v>106</v>
       </c>
       <c r="C41" s="39" t="s">
@@ -3191,8 +3317,8 @@
       <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="53"/>
-      <c r="B42" s="59"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="39" t="s">
         <v>100</v>
       </c>
@@ -3220,8 +3346,8 @@
       <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="53"/>
-      <c r="B43" s="59"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="41" t="s">
         <v>101</v>
       </c>
@@ -3249,8 +3375,8 @@
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="53"/>
-      <c r="B44" s="59"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="42" t="s">
         <v>101</v>
       </c>
@@ -3278,8 +3404,8 @@
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="54"/>
-      <c r="B45" s="60"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="41" t="s">
         <v>109</v>
       </c>
@@ -3307,10 +3433,10 @@
       <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="50" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="42" t="s">
@@ -3340,8 +3466,8 @@
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="54"/>
-      <c r="B47" s="60"/>
+      <c r="A47" s="68"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="42" t="s">
         <v>103</v>
       </c>
@@ -3369,10 +3495,10 @@
       <c r="S47" s="1"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="52" t="s">
+      <c r="A48" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="50" t="s">
         <v>108</v>
       </c>
       <c r="C48" s="39" t="s">
@@ -3402,8 +3528,8 @@
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="54"/>
-      <c r="B49" s="60"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="51"/>
       <c r="C49" s="39" t="s">
         <v>105</v>
       </c>
@@ -3431,14 +3557,14 @@
       <c r="S49" s="1"/>
     </row>
     <row r="50" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50" s="55" t="s">
-        <v>141</v>
+      <c r="A50" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="61" t="s">
+        <v>138</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D50" s="29">
         <v>1</v>
@@ -3464,10 +3590,10 @@
       <c r="S50" s="1"/>
     </row>
     <row r="51" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="62"/>
-      <c r="B51" s="56"/>
+      <c r="A51" s="64"/>
+      <c r="B51" s="69"/>
       <c r="C51" s="38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D51" s="29">
         <v>1</v>
@@ -3493,10 +3619,10 @@
       <c r="S51" s="1"/>
     </row>
     <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="63"/>
-      <c r="B52" s="57"/>
+      <c r="A52" s="65"/>
+      <c r="B52" s="62"/>
       <c r="C52" s="39" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D52" s="29">
         <v>0.5</v>
@@ -3522,14 +3648,14 @@
       <c r="S52" s="1"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="52" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" s="58" t="s">
-        <v>142</v>
+      <c r="A53" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="50" t="s">
+        <v>139</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D53" s="44">
         <v>1</v>
@@ -3555,10 +3681,10 @@
       <c r="S53" s="1"/>
     </row>
     <row r="54" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="53"/>
-      <c r="B54" s="59"/>
+      <c r="A54" s="67"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="39" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D54" s="35">
         <v>2</v>
@@ -3584,10 +3710,10 @@
       <c r="S54" s="1"/>
     </row>
     <row r="55" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="53"/>
-      <c r="B55" s="59"/>
+      <c r="A55" s="67"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D55" s="35">
         <v>2</v>
@@ -3613,10 +3739,10 @@
       <c r="S55" s="1"/>
     </row>
     <row r="56" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="53"/>
-      <c r="B56" s="59"/>
+      <c r="A56" s="67"/>
+      <c r="B56" s="52"/>
       <c r="C56" s="42" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D56" s="35">
         <v>2</v>
@@ -3642,10 +3768,10 @@
       <c r="S56" s="1"/>
     </row>
     <row r="57" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="54"/>
-      <c r="B57" s="60"/>
+      <c r="A57" s="68"/>
+      <c r="B57" s="51"/>
       <c r="C57" s="41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D57" s="35">
         <v>3</v>
@@ -3671,14 +3797,14 @@
       <c r="S57" s="1"/>
     </row>
     <row r="58" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" s="58" t="s">
-        <v>143</v>
+      <c r="A58" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>140</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D58" s="35">
         <v>1</v>
@@ -3704,10 +3830,10 @@
       <c r="S58" s="1"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="54"/>
-      <c r="B59" s="60"/>
+      <c r="A59" s="68"/>
+      <c r="B59" s="51"/>
       <c r="C59" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D59" s="35">
         <v>3</v>
@@ -3733,14 +3859,14 @@
       <c r="S59" s="1"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B60" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="C60" s="49" t="s">
-        <v>128</v>
+      <c r="A60" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" s="46" t="s">
+        <v>125</v>
       </c>
       <c r="D60" s="35">
         <v>2</v>
@@ -3766,10 +3892,10 @@
       <c r="S60" s="1"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="53"/>
-      <c r="B61" s="56"/>
+      <c r="A61" s="67"/>
+      <c r="B61" s="69"/>
       <c r="C61" s="42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D61" s="35">
         <v>1.5</v>
@@ -3795,10 +3921,10 @@
       <c r="S61" s="1"/>
     </row>
     <row r="62" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="53"/>
-      <c r="B62" s="56"/>
+      <c r="A62" s="67"/>
+      <c r="B62" s="69"/>
       <c r="C62" s="39" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D62" s="35">
         <v>2</v>
@@ -3824,10 +3950,10 @@
       <c r="S62" s="1"/>
     </row>
     <row r="63" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="53"/>
-      <c r="B63" s="56"/>
+      <c r="A63" s="67"/>
+      <c r="B63" s="69"/>
       <c r="C63" s="39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D63" s="35">
         <v>1</v>
@@ -3853,10 +3979,10 @@
       <c r="S63" s="1"/>
     </row>
     <row r="64" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="53"/>
-      <c r="B64" s="56"/>
+      <c r="A64" s="67"/>
+      <c r="B64" s="69"/>
       <c r="C64" s="39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D64" s="35">
         <v>1.5</v>
@@ -3882,10 +4008,10 @@
       <c r="S64" s="1"/>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="53"/>
-      <c r="B65" s="56"/>
+      <c r="A65" s="67"/>
+      <c r="B65" s="69"/>
       <c r="C65" s="39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D65" s="35">
         <v>1.5</v>
@@ -3911,10 +4037,10 @@
       <c r="S65" s="1"/>
     </row>
     <row r="66" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="53"/>
-      <c r="B66" s="56"/>
+      <c r="A66" s="67"/>
+      <c r="B66" s="69"/>
       <c r="C66" s="39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D66" s="35">
         <v>2</v>
@@ -3940,10 +4066,10 @@
       <c r="S66" s="1"/>
     </row>
     <row r="67" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="53"/>
-      <c r="B67" s="56"/>
+      <c r="A67" s="67"/>
+      <c r="B67" s="69"/>
       <c r="C67" s="39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D67" s="35">
         <v>2</v>
@@ -3969,10 +4095,10 @@
       <c r="S67" s="1"/>
     </row>
     <row r="68" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="53"/>
-      <c r="B68" s="56"/>
+      <c r="A68" s="67"/>
+      <c r="B68" s="69"/>
       <c r="C68" s="39" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D68" s="35">
         <v>2</v>
@@ -3998,10 +4124,10 @@
       <c r="S68" s="1"/>
     </row>
     <row r="69" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="53"/>
-      <c r="B69" s="57"/>
+      <c r="A69" s="67"/>
+      <c r="B69" s="62"/>
       <c r="C69" s="39" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D69" s="35">
         <v>2</v>
@@ -4027,14 +4153,14 @@
       <c r="S69" s="1"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B70" s="58" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="50" t="s">
-        <v>138</v>
+      <c r="A70" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="B70" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="47" t="s">
+        <v>135</v>
       </c>
       <c r="D70" s="35">
         <v>2</v>
@@ -4060,10 +4186,10 @@
       <c r="S70" s="1"/>
     </row>
     <row r="71" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="53"/>
-      <c r="B71" s="59"/>
+      <c r="A71" s="67"/>
+      <c r="B71" s="52"/>
       <c r="C71" s="39" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D71" s="35">
         <v>3</v>
@@ -4089,10 +4215,10 @@
       <c r="S71" s="1"/>
     </row>
     <row r="72" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="54"/>
-      <c r="B72" s="60"/>
+      <c r="A72" s="68"/>
+      <c r="B72" s="51"/>
       <c r="C72" s="39" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D72" s="35">
         <v>3</v>
@@ -4118,11 +4244,11 @@
       <c r="S72" s="1"/>
     </row>
     <row r="73" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="B73" s="58" t="s">
-        <v>146</v>
+      <c r="A73" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" s="50" t="s">
+        <v>143</v>
       </c>
       <c r="C73" s="33" t="s">
         <v>96</v>
@@ -4151,8 +4277,8 @@
       <c r="S73" s="1"/>
     </row>
     <row r="74" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="53"/>
-      <c r="B74" s="59"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="52"/>
       <c r="C74" s="38" t="s">
         <v>97</v>
       </c>
@@ -4180,8 +4306,8 @@
       <c r="S74" s="1"/>
     </row>
     <row r="75" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="54"/>
-      <c r="B75" s="60"/>
+      <c r="A75" s="68"/>
+      <c r="B75" s="51"/>
       <c r="C75" s="39" t="s">
         <v>98</v>
       </c>
@@ -4209,12 +4335,24 @@
       <c r="S75" s="1"/>
     </row>
     <row r="76" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="47"/>
-      <c r="B76" s="46"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="6"/>
+      <c r="A76" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="29">
+        <v>1</v>
+      </c>
+      <c r="E76" s="29">
+        <v>1</v>
+      </c>
+      <c r="F76" s="6">
+        <v>8</v>
+      </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
@@ -4230,12 +4368,20 @@
       <c r="S76" s="1"/>
     </row>
     <row r="77" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="47"/>
-      <c r="B77" s="46"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="6"/>
+      <c r="A77" s="64"/>
+      <c r="B77" s="52"/>
+      <c r="C77" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="29">
+        <v>1</v>
+      </c>
+      <c r="E77" s="29">
+        <v>1</v>
+      </c>
+      <c r="F77" s="6">
+        <v>8</v>
+      </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
@@ -4251,12 +4397,20 @@
       <c r="S77" s="1"/>
     </row>
     <row r="78" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="47"/>
-      <c r="B78" s="46"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="6"/>
+      <c r="A78" s="65"/>
+      <c r="B78" s="51"/>
+      <c r="C78" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D78" s="29">
+        <v>2</v>
+      </c>
+      <c r="E78" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="F78" s="6">
+        <v>8</v>
+      </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -4272,14 +4426,24 @@
       <c r="S78" s="1"/>
     </row>
     <row r="79" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="B79" s="46"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="6"/>
+      <c r="A79" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="C79" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D79" s="43">
+        <v>2</v>
+      </c>
+      <c r="E79" s="44">
+        <v>2</v>
+      </c>
+      <c r="F79" s="6">
+        <v>8</v>
+      </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -4295,14 +4459,20 @@
       <c r="S79" s="1"/>
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B80" s="46"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
-      <c r="F80" s="6"/>
+      <c r="A80" s="67"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="35">
+        <v>2</v>
+      </c>
+      <c r="E80" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="F80" s="6">
+        <v>8</v>
+      </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -4318,14 +4488,20 @@
       <c r="S80" s="1"/>
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="B81" s="46"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="35"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="6"/>
+      <c r="A81" s="67"/>
+      <c r="B81" s="52"/>
+      <c r="C81" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D81" s="35">
+        <v>1</v>
+      </c>
+      <c r="E81" s="35">
+        <v>1</v>
+      </c>
+      <c r="F81" s="6">
+        <v>8</v>
+      </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -4341,12 +4517,20 @@
       <c r="S81" s="1"/>
     </row>
     <row r="82" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="47"/>
-      <c r="B82" s="46"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="6"/>
+      <c r="A82" s="67"/>
+      <c r="B82" s="52"/>
+      <c r="C82" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" s="35">
+        <v>3</v>
+      </c>
+      <c r="E82" s="35">
+        <v>2.5</v>
+      </c>
+      <c r="F82" s="6">
+        <v>8</v>
+      </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
@@ -4362,12 +4546,20 @@
       <c r="S82" s="1"/>
     </row>
     <row r="83" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="47"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="35"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="6"/>
+      <c r="A83" s="68"/>
+      <c r="B83" s="51"/>
+      <c r="C83" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D83" s="35">
+        <v>2</v>
+      </c>
+      <c r="E83" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="F83" s="6">
+        <v>8</v>
+      </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
@@ -4382,13 +4574,25 @@
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
     </row>
-    <row r="84" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="45"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="6"/>
+    <row r="84" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D84" s="35">
+        <v>2</v>
+      </c>
+      <c r="E84" s="35">
+        <v>1.25</v>
+      </c>
+      <c r="F84" s="6">
+        <v>8</v>
+      </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -4403,13 +4607,21 @@
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
     </row>
-    <row r="85" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="45"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
-      <c r="F85" s="6"/>
+    <row r="85" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="67"/>
+      <c r="B85" s="52"/>
+      <c r="C85" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="D85" s="35">
+        <v>2</v>
+      </c>
+      <c r="E85" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="F85" s="6">
+        <v>8</v>
+      </c>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -4424,13 +4636,21 @@
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
     </row>
-    <row r="86" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="45"/>
-      <c r="B86" s="37"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="6"/>
+    <row r="86" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="67"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D86" s="35">
+        <v>1</v>
+      </c>
+      <c r="E86" s="35">
+        <v>1</v>
+      </c>
+      <c r="F86" s="6">
+        <v>8</v>
+      </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -4445,13 +4665,21 @@
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
     </row>
-    <row r="87" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="45"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="6"/>
+    <row r="87" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="67"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="D87" s="35">
+        <v>1</v>
+      </c>
+      <c r="E87" s="35">
+        <v>1</v>
+      </c>
+      <c r="F87" s="6">
+        <v>8</v>
+      </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -4466,13 +4694,21 @@
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
     </row>
-    <row r="88" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="51"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="6"/>
+    <row r="88" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="67"/>
+      <c r="B88" s="52"/>
+      <c r="C88" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="D88" s="35">
+        <v>1</v>
+      </c>
+      <c r="E88" s="35">
+        <v>1</v>
+      </c>
+      <c r="F88" s="6">
+        <v>8</v>
+      </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -4487,13 +4723,21 @@
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
     </row>
-    <row r="89" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="51"/>
-      <c r="B89" s="37"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="35"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="6"/>
+    <row r="89" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="67"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="D89" s="35">
+        <v>1</v>
+      </c>
+      <c r="E89" s="35">
+        <v>1</v>
+      </c>
+      <c r="F89" s="6">
+        <v>8</v>
+      </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -4508,13 +4752,21 @@
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
     </row>
-    <row r="90" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="51"/>
-      <c r="B90" s="37"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="6"/>
+    <row r="90" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="67"/>
+      <c r="B90" s="52"/>
+      <c r="C90" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" s="35">
+        <v>1</v>
+      </c>
+      <c r="E90" s="35">
+        <v>1</v>
+      </c>
+      <c r="F90" s="6">
+        <v>8</v>
+      </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -4529,13 +4781,21 @@
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
     </row>
-    <row r="91" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="45"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="28"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="6"/>
+    <row r="91" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="67"/>
+      <c r="B91" s="52"/>
+      <c r="C91" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="D91" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="E91" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="F91" s="6">
+        <v>8</v>
+      </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -4550,15 +4810,21 @@
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
     </row>
-    <row r="92" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="67"/>
+      <c r="B92" s="52"/>
+      <c r="C92" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="D92" s="35">
+        <v>1</v>
+      </c>
+      <c r="E92" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F92" s="6">
         <v>8</v>
       </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="9"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -4573,13 +4839,21 @@
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
     </row>
-    <row r="93" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="7"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="6"/>
+    <row r="93" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="67"/>
+      <c r="B93" s="52"/>
+      <c r="C93" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="D93" s="35">
+        <v>1</v>
+      </c>
+      <c r="E93" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F93" s="6">
+        <v>8</v>
+      </c>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
@@ -4594,13 +4868,21 @@
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
     </row>
-    <row r="94" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="6"/>
+    <row r="94" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67"/>
+      <c r="B94" s="52"/>
+      <c r="C94" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D94" s="35">
+        <v>1</v>
+      </c>
+      <c r="E94" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F94" s="6">
+        <v>8</v>
+      </c>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -4615,15 +4897,21 @@
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
     </row>
-    <row r="95" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="9"/>
+    <row r="95" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="67"/>
+      <c r="B95" s="52"/>
+      <c r="C95" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="E95" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="F95" s="6">
+        <v>8</v>
+      </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
@@ -4638,13 +4926,21 @@
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
     </row>
-    <row r="96" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="6"/>
+    <row r="96" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="67"/>
+      <c r="B96" s="52"/>
+      <c r="C96" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D96" s="35">
+        <v>1</v>
+      </c>
+      <c r="E96" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F96" s="6">
+        <v>8</v>
+      </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
@@ -4659,13 +4955,21 @@
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
     </row>
-    <row r="97" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="6"/>
+    <row r="97" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="67"/>
+      <c r="B97" s="52"/>
+      <c r="C97" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="D97" s="35">
+        <v>1</v>
+      </c>
+      <c r="E97" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F97" s="6">
+        <v>8</v>
+      </c>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
@@ -4680,21 +4984,21 @@
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
     </row>
-    <row r="98" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A98" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="11">
-        <f>SUM(D4:D97)</f>
-        <v>229.52999999999997</v>
-      </c>
-      <c r="E98" s="11">
-        <f>SUM(E4:E97)</f>
-        <v>228.72999999999996</v>
-      </c>
-      <c r="F98" s="6"/>
+    <row r="98" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="67"/>
+      <c r="B98" s="52"/>
+      <c r="C98" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D98" s="35">
+        <v>1</v>
+      </c>
+      <c r="E98" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F98" s="6">
+        <v>8</v>
+      </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
@@ -4709,40 +5013,1015 @@
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="E99" s="26"/>
+    <row r="99" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="67"/>
+      <c r="B99" s="52"/>
+      <c r="C99" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="D99" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="E99" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="F99" s="6">
+        <v>8</v>
+      </c>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+    </row>
+    <row r="100" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="67"/>
+      <c r="B100" s="52"/>
+      <c r="C100" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="D100" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E100" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F100" s="6">
+        <v>8</v>
+      </c>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+    </row>
+    <row r="101" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="67"/>
+      <c r="B101" s="52"/>
+      <c r="C101" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D101" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E101" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F101" s="6">
+        <v>8</v>
+      </c>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+    </row>
+    <row r="102" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="67"/>
+      <c r="B102" s="52"/>
+      <c r="C102" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D102" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E102" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F102" s="6">
+        <v>8</v>
+      </c>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+    </row>
+    <row r="103" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="67"/>
+      <c r="B103" s="52"/>
+      <c r="C103" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="D103" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E103" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F103" s="6">
+        <v>8</v>
+      </c>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+    </row>
+    <row r="104" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="67"/>
+      <c r="B104" s="52"/>
+      <c r="C104" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="D104" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E104" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F104" s="6">
+        <v>8</v>
+      </c>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+    </row>
+    <row r="105" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="67"/>
+      <c r="B105" s="52"/>
+      <c r="C105" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="D105" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E105" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F105" s="6">
+        <v>8</v>
+      </c>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+    </row>
+    <row r="106" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="67"/>
+      <c r="B106" s="52"/>
+      <c r="C106" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="D106" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E106" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F106" s="6">
+        <v>8</v>
+      </c>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="1"/>
+    </row>
+    <row r="107" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="67"/>
+      <c r="B107" s="52"/>
+      <c r="C107" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D107" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E107" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F107" s="6">
+        <v>8</v>
+      </c>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+      <c r="R107" s="1"/>
+      <c r="S107" s="1"/>
+    </row>
+    <row r="108" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="67"/>
+      <c r="B108" s="52"/>
+      <c r="C108" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D108" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E108" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F108" s="6">
+        <v>8</v>
+      </c>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+      <c r="S108" s="1"/>
+    </row>
+    <row r="109" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="67"/>
+      <c r="B109" s="52"/>
+      <c r="C109" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="D109" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E109" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F109" s="6">
+        <v>8</v>
+      </c>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+      <c r="S109" s="1"/>
+    </row>
+    <row r="110" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="67"/>
+      <c r="B110" s="52"/>
+      <c r="C110" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="D110" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E110" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F110" s="6">
+        <v>8</v>
+      </c>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="1"/>
+      <c r="S110" s="1"/>
+    </row>
+    <row r="111" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="67"/>
+      <c r="B111" s="52"/>
+      <c r="C111" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D111" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E111" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F111" s="6">
+        <v>8</v>
+      </c>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1"/>
+      <c r="P111" s="1"/>
+      <c r="Q111" s="1"/>
+      <c r="R111" s="1"/>
+      <c r="S111" s="1"/>
+    </row>
+    <row r="112" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="67"/>
+      <c r="B112" s="52"/>
+      <c r="C112" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="D112" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E112" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F112" s="6">
+        <v>8</v>
+      </c>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="1"/>
+      <c r="S112" s="1"/>
+    </row>
+    <row r="113" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="68"/>
+      <c r="B113" s="51"/>
+      <c r="C113" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D113" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E113" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F113" s="6">
+        <v>8</v>
+      </c>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="1"/>
+      <c r="S113" s="1"/>
+    </row>
+    <row r="114" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="B114" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D114" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="E114" s="35">
+        <v>2</v>
+      </c>
+      <c r="F114" s="6">
+        <v>8</v>
+      </c>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1"/>
+      <c r="R114" s="1"/>
+      <c r="S114" s="1"/>
+    </row>
+    <row r="115" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="67"/>
+      <c r="B115" s="52"/>
+      <c r="C115" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="D115" s="35">
+        <v>2</v>
+      </c>
+      <c r="E115" s="35">
+        <v>2</v>
+      </c>
+      <c r="F115" s="6">
+        <v>8</v>
+      </c>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+      <c r="P115" s="1"/>
+      <c r="Q115" s="1"/>
+      <c r="R115" s="1"/>
+      <c r="S115" s="1"/>
+    </row>
+    <row r="116" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="68"/>
+      <c r="B116" s="51"/>
+      <c r="C116" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D116" s="35">
+        <v>1</v>
+      </c>
+      <c r="E116" s="35">
+        <v>1</v>
+      </c>
+      <c r="F116" s="6">
+        <v>8</v>
+      </c>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
+      <c r="P116" s="1"/>
+      <c r="Q116" s="1"/>
+      <c r="R116" s="1"/>
+      <c r="S116" s="1"/>
+    </row>
+    <row r="117" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B117" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C117" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D117" s="35">
+        <v>2</v>
+      </c>
+      <c r="E117" s="35">
+        <v>2</v>
+      </c>
+      <c r="F117" s="6">
+        <v>8</v>
+      </c>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+      <c r="P117" s="1"/>
+      <c r="Q117" s="1"/>
+      <c r="R117" s="1"/>
+      <c r="S117" s="1"/>
+    </row>
+    <row r="118" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="67"/>
+      <c r="B118" s="52"/>
+      <c r="C118" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D118" s="35">
+        <v>2</v>
+      </c>
+      <c r="E118" s="35">
+        <v>3</v>
+      </c>
+      <c r="F118" s="6">
+        <v>8</v>
+      </c>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+      <c r="P118" s="1"/>
+      <c r="Q118" s="1"/>
+      <c r="R118" s="1"/>
+      <c r="S118" s="1"/>
+    </row>
+    <row r="119" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="67"/>
+      <c r="B119" s="52"/>
+      <c r="C119" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D119" s="35">
+        <v>3</v>
+      </c>
+      <c r="E119" s="35">
+        <v>3</v>
+      </c>
+      <c r="F119" s="6">
+        <v>8</v>
+      </c>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1"/>
+      <c r="P119" s="1"/>
+      <c r="Q119" s="1"/>
+      <c r="R119" s="1"/>
+      <c r="S119" s="1"/>
+    </row>
+    <row r="120" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="67"/>
+      <c r="B120" s="51"/>
+      <c r="C120" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="D120" s="35">
+        <v>1</v>
+      </c>
+      <c r="E120" s="35">
+        <v>1</v>
+      </c>
+      <c r="F120" s="6">
+        <v>8</v>
+      </c>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+      <c r="P120" s="1"/>
+      <c r="Q120" s="1"/>
+      <c r="R120" s="1"/>
+      <c r="S120" s="1"/>
+    </row>
+    <row r="121" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A121" s="48"/>
+      <c r="B121" s="49"/>
+      <c r="C121" s="39"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="35"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1"/>
+      <c r="P121" s="1"/>
+      <c r="Q121" s="1"/>
+      <c r="R121" s="1"/>
+      <c r="S121" s="1"/>
+    </row>
+    <row r="122" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A122" s="48"/>
+      <c r="B122" s="49"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="35"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+      <c r="P122" s="1"/>
+      <c r="Q122" s="1"/>
+      <c r="R122" s="1"/>
+      <c r="S122" s="1"/>
+    </row>
+    <row r="123" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A123" s="48"/>
+      <c r="B123" s="49"/>
+      <c r="C123" s="39"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="35"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+      <c r="O123" s="1"/>
+      <c r="P123" s="1"/>
+      <c r="Q123" s="1"/>
+      <c r="R123" s="1"/>
+      <c r="S123" s="1"/>
+    </row>
+    <row r="124" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A124" s="48"/>
+      <c r="B124" s="49"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="35"/>
+      <c r="E124" s="35"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+      <c r="N124" s="1"/>
+      <c r="O124" s="1"/>
+      <c r="P124" s="1"/>
+      <c r="Q124" s="1"/>
+      <c r="R124" s="1"/>
+      <c r="S124" s="1"/>
+    </row>
+    <row r="125" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A125" s="48"/>
+      <c r="B125" s="49"/>
+      <c r="C125" s="39"/>
+      <c r="D125" s="35"/>
+      <c r="E125" s="35"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1"/>
+      <c r="P125" s="1"/>
+      <c r="Q125" s="1"/>
+      <c r="R125" s="1"/>
+      <c r="S125" s="1"/>
+    </row>
+    <row r="126" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A126" s="48"/>
+      <c r="B126" s="49"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="35"/>
+      <c r="E126" s="35"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1"/>
+      <c r="R126" s="1"/>
+      <c r="S126" s="1"/>
+    </row>
+    <row r="127" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A127" s="48"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="39"/>
+      <c r="D127" s="35"/>
+      <c r="E127" s="35"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+      <c r="N127" s="1"/>
+      <c r="O127" s="1"/>
+      <c r="P127" s="1"/>
+      <c r="Q127" s="1"/>
+      <c r="R127" s="1"/>
+      <c r="S127" s="1"/>
+    </row>
+    <row r="128" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A128" s="48"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="39"/>
+      <c r="D128" s="35"/>
+      <c r="E128" s="35"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+      <c r="L128" s="1"/>
+      <c r="M128" s="1"/>
+      <c r="N128" s="1"/>
+      <c r="O128" s="1"/>
+      <c r="P128" s="1"/>
+      <c r="Q128" s="1"/>
+      <c r="R128" s="1"/>
+      <c r="S128" s="1"/>
+    </row>
+    <row r="129" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="45"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="28"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+      <c r="L129" s="1"/>
+      <c r="M129" s="1"/>
+      <c r="N129" s="1"/>
+      <c r="O129" s="1"/>
+      <c r="P129" s="1"/>
+      <c r="Q129" s="1"/>
+      <c r="R129" s="1"/>
+      <c r="S129" s="1"/>
+    </row>
+    <row r="130" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="36"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="M130" s="1"/>
+      <c r="N130" s="1"/>
+      <c r="O130" s="1"/>
+      <c r="P130" s="1"/>
+      <c r="Q130" s="1"/>
+      <c r="R130" s="1"/>
+      <c r="S130" s="1"/>
+    </row>
+    <row r="131" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A131" s="7"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
+      <c r="O131" s="1"/>
+      <c r="P131" s="1"/>
+      <c r="Q131" s="1"/>
+      <c r="R131" s="1"/>
+      <c r="S131" s="1"/>
+    </row>
+    <row r="132" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+      <c r="Q132" s="1"/>
+      <c r="R132" s="1"/>
+      <c r="S132" s="1"/>
+    </row>
+    <row r="133" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="P133" s="1"/>
+      <c r="Q133" s="1"/>
+      <c r="R133" s="1"/>
+      <c r="S133" s="1"/>
+    </row>
+    <row r="134" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+      <c r="Q134" s="1"/>
+      <c r="R134" s="1"/>
+      <c r="S134" s="1"/>
+    </row>
+    <row r="135" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+      <c r="Q135" s="1"/>
+      <c r="R135" s="1"/>
+      <c r="S135" s="1"/>
+    </row>
+    <row r="136" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A136" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136" s="4"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="11">
+        <f>SUM(D4:D135)</f>
+        <v>276.39999999999975</v>
+      </c>
+      <c r="E136" s="11">
+        <f>SUM(E4:E135)</f>
+        <v>273.47999999999996</v>
+      </c>
+      <c r="F136" s="6"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
+      <c r="N136" s="1"/>
+      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
+      <c r="Q136" s="1"/>
+      <c r="R136" s="1"/>
+      <c r="S136" s="1"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E137" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="B8:B14"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
+  <mergeCells count="51">
+    <mergeCell ref="A84:A113"/>
+    <mergeCell ref="B84:B113"/>
+    <mergeCell ref="A114:A116"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="B79:B83"/>
     <mergeCell ref="A73:A75"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="B53:B57"/>
@@ -4755,6 +6034,35 @@
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A60:A69"/>
     <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -4790,20 +6098,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74" t="s">
+      <c r="A1" s="73"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
       <c r="O1" s="1"/>
@@ -4818,40 +6126,40 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="70" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="1"/>
@@ -4866,18 +6174,18 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="75"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -5015,15 +6323,15 @@
       </c>
       <c r="J6" s="18">
         <f t="shared" si="1"/>
-        <v>271.27</v>
+        <v>226.51999999999998</v>
       </c>
       <c r="K6" s="18">
         <f t="shared" si="1"/>
-        <v>271.27</v>
+        <v>226.51999999999998</v>
       </c>
       <c r="L6" s="18">
         <f t="shared" si="1"/>
-        <v>271.27</v>
+        <v>226.51999999999998</v>
       </c>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
@@ -5065,22 +6373,22 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
       <c r="M8" s="20" t="s">
         <v>10</v>
       </c>
@@ -5099,10 +6407,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="73">
+      <c r="A9" s="72">
         <v>50</v>
       </c>
-      <c r="B9" s="73"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="18">
         <f>SUMIF('Product Backlog'!F:F,1,'Product Backlog'!E:E)</f>
         <v>39</v>
@@ -5133,7 +6441,7 @@
       </c>
       <c r="J9" s="18">
         <f>SUMIF('Product Backlog'!F:F,8,'Product Backlog'!E:E)</f>
-        <v>0</v>
+        <v>44.75</v>
       </c>
       <c r="K9" s="18">
         <f>SUMIF('Product Backlog'!F:F,9,'Product Backlog'!E:E)</f>
@@ -5145,11 +6453,11 @@
       </c>
       <c r="M9" s="18">
         <f>SUM(C9:L9)</f>
-        <v>228.73000000000002</v>
+        <v>273.48</v>
       </c>
       <c r="N9" s="18">
         <f>M9/10</f>
-        <v>22.873000000000001</v>
+        <v>27.348000000000003</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -5164,6 +6472,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:L8"/>
@@ -5180,7 +6489,6 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>